<commit_message>
shorter ja venue names. better fa team name fonts
</commit_message>
<xml_diff>
--- a/src/stp/database/localization.xlsx
+++ b/src/stp/database/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D186F51-0A32-1144-B78D-2E94015B1B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B3FB7F-D59A-344F-B5AA-0FA235FB7F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19760" activeTab="9" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="34200" windowHeight="19300" activeTab="2" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Competition" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1470">
   <si>
     <t>key</t>
   </si>
@@ -3862,18 +3862,12 @@
     <t>Estadio Australia</t>
   </si>
   <si>
-    <t>スタジアム・オーストラリア</t>
-  </si>
-  <si>
     <t>au-sydney_football</t>
   </si>
   <si>
     <t>Estadio de fútbol de Sídney</t>
   </si>
   <si>
-    <t>シドニー・フットボール・スタジアム</t>
-  </si>
-  <si>
     <t>ca-toronto</t>
   </si>
   <si>
@@ -3979,9 +3973,6 @@
     <t>Khalifa International</t>
   </si>
   <si>
-    <t>ハリファ・インターナショナル</t>
-  </si>
-  <si>
     <t>خلیفه بین‌المللی</t>
   </si>
   <si>
@@ -4321,9 +4312,6 @@
     <t>us-east-rutherford-nj</t>
   </si>
   <si>
-    <t>イーストラザフォード、NJ</t>
-  </si>
-  <si>
     <t>ایست رادرفورد، NJ</t>
   </si>
   <si>
@@ -4466,6 +4454,18 @@
   </si>
   <si>
     <t>واشنگتن، DC</t>
+  </si>
+  <si>
+    <t>final.team.name</t>
+  </si>
+  <si>
+    <t>シドニーSFS</t>
+  </si>
+  <si>
+    <t>ハリファ</t>
+  </si>
+  <si>
+    <t>ラザフォード、NJ</t>
   </si>
 </sst>
 </file>
@@ -4667,46 +4667,15 @@
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+          <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -4737,44 +4706,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4830,6 +4761,75 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4844,7 +4844,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00C34F16-7F53-D94E-8507-5A463D8AE41D}" name="Competition" displayName="Competition" ref="A1:I6" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00C34F16-7F53-D94E-8507-5A463D8AE41D}" name="Competition" displayName="Competition" ref="A1:I6" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:I6" xr:uid="{00C34F16-7F53-D94E-8507-5A463D8AE41D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DE8C6A4E-E5F4-7F49-B2CA-17BFBEA37A38}" name="key"/>
@@ -4862,10 +4862,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0">
-  <autoFilter ref="A1:J22" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J22">
-    <sortCondition ref="A1:A22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J23" totalsRowShown="0">
+  <autoFilter ref="A1:J23" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J23">
+    <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4614A9ED-E890-4F3B-BD19-53C40876125F}" name="key"/>
@@ -4884,7 +4884,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9C7FB29C-EA6A-4E41-8C16-FE95CB8776FE}" name="Host" displayName="Host" ref="A1:I10" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9C7FB29C-EA6A-4E41-8C16-FE95CB8776FE}" name="Host" displayName="Host" ref="A1:I10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6">
   <autoFilter ref="A1:I10" xr:uid="{9C7FB29C-EA6A-4E41-8C16-FE95CB8776FE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4C829EE4-C95B-7542-9E54-757777F7C77B}" name="key"/>
@@ -4902,7 +4902,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A92B97DC-54AE-2A49-B366-A6504207E4CF}" name="Venue" displayName="Venue" ref="A1:I71" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A92B97DC-54AE-2A49-B366-A6504207E4CF}" name="Venue" displayName="Venue" ref="A1:I71" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
   <autoFilter ref="A1:I71" xr:uid="{A92B97DC-54AE-2A49-B366-A6504207E4CF}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B0B3E3B6-7AC0-B341-AA47-E0828ED515C1}" name="key"/>
@@ -4966,7 +4966,7 @@
     <tableColumn id="5" xr3:uid="{0318B88A-79B0-4BA8-931F-32E598CDDD83}" name="fr"/>
     <tableColumn id="6" xr3:uid="{7FB94F46-D9D6-4FFA-A68A-D9C22DD62960}" name="de"/>
     <tableColumn id="7" xr3:uid="{8DA7014B-3E29-4B6A-905E-FD5A34D770FA}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{21D35627-DEB2-4E21-A7A7-5800DA843F2D}" name="ja" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{21D35627-DEB2-4E21-A7A7-5800DA843F2D}" name="ja" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{0E0ECA8B-5B6D-4A0F-9BA3-F5F697D5FD39}" name="fa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5014,10 +5014,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I42" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I42" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:I42" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E3E8593F-CDB5-CA4C-B2DF-C5D167E6F581}" name="en"/>
     <tableColumn id="3" xr3:uid="{583B6CFD-84CD-BB44-88B6-0A0D3BA2E05E}" name="es"/>
     <tableColumn id="4" xr3:uid="{3139A9B8-E0C7-184A-8291-97B79E51FC05}" name="it"/>
@@ -5516,10 +5516,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I17"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5684,61 +5684,61 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>657</v>
+        <v>1466</v>
       </c>
       <c r="B9" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C9" t="s">
         <v>670</v>
       </c>
       <c r="I9" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J9" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="B10" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I10" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>644</v>
+        <v>655</v>
       </c>
       <c r="B11" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="C11" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I11" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="J11" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B12" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C12" t="s">
         <v>670</v>
@@ -5752,109 +5752,109 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B13" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C13" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I13" t="s">
-        <v>660</v>
+        <v>673</v>
       </c>
       <c r="J13" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B14" t="s">
         <v>660</v>
       </c>
       <c r="C14" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
       <c r="I14" t="s">
         <v>660</v>
       </c>
       <c r="J14" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B15" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C15" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="I15" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="J15" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="B16" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="C16" t="s">
         <v>670</v>
       </c>
       <c r="I16" t="s">
-        <v>660</v>
+        <v>673</v>
       </c>
       <c r="J16" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1024</v>
+        <v>650</v>
       </c>
       <c r="B17" t="s">
-        <v>1025</v>
+        <v>660</v>
       </c>
       <c r="C17" t="s">
         <v>670</v>
       </c>
       <c r="I17" t="s">
-        <v>1025</v>
+        <v>660</v>
       </c>
       <c r="J17" t="s">
-        <v>1025</v>
+        <v>660</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>651</v>
+        <v>1024</v>
       </c>
       <c r="B18" t="s">
-        <v>665</v>
+        <v>1025</v>
       </c>
       <c r="C18" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I18" t="s">
-        <v>675</v>
+        <v>1025</v>
       </c>
       <c r="J18" t="s">
-        <v>672</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>693</v>
+        <v>651</v>
       </c>
       <c r="B19" t="s">
         <v>665</v>
@@ -5871,52 +5871,69 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>649</v>
+        <v>693</v>
       </c>
       <c r="B20" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="C20" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="I20" t="s">
-        <v>660</v>
+        <v>675</v>
       </c>
       <c r="J20" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B21" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C21" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="I21" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="J21" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>648</v>
+      </c>
+      <c r="B22" t="s">
+        <v>664</v>
+      </c>
+      <c r="C22" t="s">
+        <v>670</v>
+      </c>
+      <c r="I22" t="s">
+        <v>674</v>
+      </c>
+      <c r="J22" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>659</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>667</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>672</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>675</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>672</v>
       </c>
     </row>
@@ -6251,8 +6268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A607C59C-9131-3A41-BBFB-E38E1FFB1A83}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6464,7 +6481,7 @@
         <v>1121</v>
       </c>
       <c r="H7" t="s">
-        <v>1268</v>
+        <v>340</v>
       </c>
       <c r="I7" t="s">
         <v>1122</v>
@@ -6472,13 +6489,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B8" t="s">
         <v>1095</v>
       </c>
       <c r="C8" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="D8" t="s">
         <v>1095</v>
@@ -6493,7 +6510,7 @@
         <v>1095</v>
       </c>
       <c r="H8" t="s">
-        <v>1271</v>
+        <v>1467</v>
       </c>
       <c r="I8" t="s">
         <v>1097</v>
@@ -6501,7 +6518,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="B9" t="s">
         <v>1213</v>
@@ -6530,7 +6547,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B10" t="s">
         <v>1210</v>
@@ -6559,13 +6576,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="B11" t="s">
         <v>1130</v>
       </c>
       <c r="C11" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="D11" t="s">
         <v>1131</v>
@@ -6588,7 +6605,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="B12" t="s">
         <v>1135</v>
@@ -6617,7 +6634,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B13" t="s">
         <v>1141</v>
@@ -6646,7 +6663,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B14" t="s">
         <v>1144</v>
@@ -6675,13 +6692,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B15" t="s">
         <v>1147</v>
       </c>
       <c r="C15" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="D15" t="s">
         <v>1149</v>
@@ -6704,7 +6721,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="B16" t="s">
         <v>1152</v>
@@ -6733,7 +6750,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="B17" t="s">
         <v>1155</v>
@@ -6762,7 +6779,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="B18" t="s">
         <v>1161</v>
@@ -6791,13 +6808,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B19" t="s">
         <v>1165</v>
       </c>
       <c r="C19" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="D19" t="s">
         <v>1166</v>
@@ -6820,7 +6837,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="B20" t="s">
         <v>1170</v>
@@ -6849,7 +6866,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B21" t="s">
         <v>1223</v>
@@ -6878,7 +6895,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="B22" t="s">
         <v>1216</v>
@@ -6907,7 +6924,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="B23" t="s">
         <v>880</v>
@@ -6936,7 +6953,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B24" t="s">
         <v>1092</v>
@@ -6965,7 +6982,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B25" t="s">
         <v>1098</v>
@@ -6994,7 +7011,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="B26" t="s">
         <v>1107</v>
@@ -7023,7 +7040,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="B27" t="s">
         <v>1104</v>
@@ -7052,7 +7069,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B28" t="s">
         <v>1068</v>
@@ -7081,7 +7098,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="B29" t="s">
         <v>1062</v>
@@ -7110,7 +7127,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B30" t="s">
         <v>1059</v>
@@ -7131,15 +7148,15 @@
         <v>1059</v>
       </c>
       <c r="H30" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="I30" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="B31" t="s">
         <v>1077</v>
@@ -7163,12 +7180,12 @@
         <v>1078</v>
       </c>
       <c r="I31" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="B32" t="s">
         <v>1060</v>
@@ -7192,12 +7209,12 @@
         <v>1061</v>
       </c>
       <c r="I32" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B33" t="s">
         <v>1075</v>
@@ -7218,7 +7235,7 @@
         <v>1075</v>
       </c>
       <c r="H33" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="I33" t="s">
         <v>1076</v>
@@ -7226,36 +7243,36 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1468</v>
+      </c>
+      <c r="I34" t="s">
         <v>1305</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="G34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="H34" t="s">
-        <v>1307</v>
-      </c>
-      <c r="I34" t="s">
-        <v>1308</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="B35" t="s">
         <v>1065</v>
@@ -7284,152 +7301,152 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E36" t="s">
         <v>1310</v>
       </c>
-      <c r="B36" t="s">
+      <c r="F36" t="s">
         <v>1311</v>
       </c>
-      <c r="C36" t="s">
+      <c r="G36" t="s">
         <v>1312</v>
       </c>
-      <c r="D36" t="s">
-        <v>1311</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="H36" t="s">
         <v>1313</v>
       </c>
-      <c r="F36" t="s">
+      <c r="I36" t="s">
         <v>1314</v>
-      </c>
-      <c r="G36" t="s">
-        <v>1315</v>
-      </c>
-      <c r="H36" t="s">
-        <v>1316</v>
-      </c>
-      <c r="I36" t="s">
-        <v>1317</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1316</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1316</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1316</v>
+      </c>
+      <c r="H37" t="s">
         <v>1318</v>
       </c>
-      <c r="B37" t="s">
+      <c r="I37" t="s">
         <v>1319</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1320</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1319</v>
-      </c>
-      <c r="E37" t="s">
-        <v>1319</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1319</v>
-      </c>
-      <c r="G37" t="s">
-        <v>1319</v>
-      </c>
-      <c r="H37" t="s">
-        <v>1321</v>
-      </c>
-      <c r="I37" t="s">
-        <v>1322</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1321</v>
+      </c>
+      <c r="F38" t="s">
         <v>1323</v>
       </c>
-      <c r="B38" t="s">
+      <c r="G38" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H38" t="s">
         <v>1324</v>
       </c>
-      <c r="C38" t="s">
+      <c r="I38" t="s">
         <v>1325</v>
-      </c>
-      <c r="D38" t="s">
-        <v>1324</v>
-      </c>
-      <c r="E38" t="s">
-        <v>1324</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1326</v>
-      </c>
-      <c r="G38" t="s">
-        <v>1324</v>
-      </c>
-      <c r="H38" t="s">
-        <v>1327</v>
-      </c>
-      <c r="I38" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D39" t="s">
         <v>1329</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
         <v>1330</v>
       </c>
-      <c r="C39" t="s">
+      <c r="F39" t="s">
         <v>1331</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
         <v>1332</v>
       </c>
-      <c r="E39" t="s">
+      <c r="H39" t="s">
         <v>1333</v>
       </c>
-      <c r="F39" t="s">
+      <c r="I39" t="s">
         <v>1334</v>
-      </c>
-      <c r="G39" t="s">
-        <v>1335</v>
-      </c>
-      <c r="H39" t="s">
-        <v>1336</v>
-      </c>
-      <c r="I39" t="s">
-        <v>1337</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
       <c r="B40" t="s">
         <v>1079</v>
       </c>
       <c r="C40" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F40" t="s">
         <v>1339</v>
       </c>
-      <c r="D40" t="s">
+      <c r="G40" t="s">
         <v>1340</v>
       </c>
-      <c r="E40" t="s">
+      <c r="H40" t="s">
         <v>1341</v>
       </c>
-      <c r="F40" t="s">
+      <c r="I40" t="s">
         <v>1342</v>
-      </c>
-      <c r="G40" t="s">
-        <v>1343</v>
-      </c>
-      <c r="H40" t="s">
-        <v>1344</v>
-      </c>
-      <c r="I40" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="B41" t="s">
         <v>1080</v>
@@ -7450,218 +7467,218 @@
         <v>1080</v>
       </c>
       <c r="H41" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="I41" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D42" t="s">
         <v>1349</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E42" t="s">
         <v>1350</v>
       </c>
-      <c r="C42" t="s">
+      <c r="F42" t="s">
         <v>1351</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>1352</v>
       </c>
-      <c r="E42" t="s">
+      <c r="H42" t="s">
         <v>1353</v>
       </c>
-      <c r="F42" t="s">
+      <c r="I42" t="s">
         <v>1354</v>
-      </c>
-      <c r="G42" t="s">
-        <v>1355</v>
-      </c>
-      <c r="H42" t="s">
-        <v>1356</v>
-      </c>
-      <c r="I42" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D43" t="s">
         <v>1358</v>
       </c>
-      <c r="B43" t="s">
+      <c r="E43" t="s">
         <v>1359</v>
       </c>
-      <c r="C43" t="s">
+      <c r="F43" t="s">
         <v>1360</v>
       </c>
-      <c r="D43" t="s">
+      <c r="G43" t="s">
         <v>1361</v>
       </c>
-      <c r="E43" t="s">
+      <c r="H43" t="s">
         <v>1362</v>
       </c>
-      <c r="F43" t="s">
+      <c r="I43" t="s">
         <v>1363</v>
-      </c>
-      <c r="G43" t="s">
-        <v>1364</v>
-      </c>
-      <c r="H43" t="s">
-        <v>1365</v>
-      </c>
-      <c r="I43" t="s">
-        <v>1366</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D44" t="s">
         <v>1367</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
         <v>1368</v>
       </c>
-      <c r="C44" t="s">
+      <c r="F44" t="s">
         <v>1369</v>
       </c>
-      <c r="D44" t="s">
+      <c r="G44" t="s">
         <v>1370</v>
       </c>
-      <c r="E44" t="s">
+      <c r="H44" t="s">
         <v>1371</v>
       </c>
-      <c r="F44" t="s">
+      <c r="I44" t="s">
         <v>1372</v>
-      </c>
-      <c r="G44" t="s">
-        <v>1373</v>
-      </c>
-      <c r="H44" t="s">
-        <v>1374</v>
-      </c>
-      <c r="I44" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1374</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1374</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1375</v>
+      </c>
+      <c r="I45" t="s">
         <v>1376</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1377</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1377</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1377</v>
-      </c>
-      <c r="E45" t="s">
-        <v>1377</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1377</v>
-      </c>
-      <c r="G45" t="s">
-        <v>1377</v>
-      </c>
-      <c r="H45" t="s">
-        <v>1378</v>
-      </c>
-      <c r="I45" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1378</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1379</v>
+      </c>
+      <c r="I46" t="s">
         <v>1380</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1381</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1381</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1381</v>
-      </c>
-      <c r="E46" t="s">
-        <v>1381</v>
-      </c>
-      <c r="F46" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G46" t="s">
-        <v>1381</v>
-      </c>
-      <c r="H46" t="s">
-        <v>1382</v>
-      </c>
-      <c r="I46" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E47" t="s">
         <v>1384</v>
       </c>
-      <c r="B47" t="s">
+      <c r="F47" t="s">
         <v>1385</v>
       </c>
-      <c r="C47" t="s">
-        <v>1385</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="G47" t="s">
         <v>1386</v>
       </c>
-      <c r="E47" t="s">
+      <c r="H47" t="s">
         <v>1387</v>
       </c>
-      <c r="F47" t="s">
+      <c r="I47" t="s">
         <v>1388</v>
-      </c>
-      <c r="G47" t="s">
-        <v>1389</v>
-      </c>
-      <c r="H47" t="s">
-        <v>1390</v>
-      </c>
-      <c r="I47" t="s">
-        <v>1391</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1390</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F48" t="s">
         <v>1392</v>
       </c>
-      <c r="B48" t="s">
+      <c r="G48" t="s">
+        <v>1392</v>
+      </c>
+      <c r="H48" t="s">
         <v>1393</v>
       </c>
-      <c r="C48" t="s">
+      <c r="I48" t="s">
         <v>1394</v>
-      </c>
-      <c r="D48" t="s">
-        <v>1393</v>
-      </c>
-      <c r="E48" t="s">
-        <v>1393</v>
-      </c>
-      <c r="F48" t="s">
-        <v>1395</v>
-      </c>
-      <c r="G48" t="s">
-        <v>1395</v>
-      </c>
-      <c r="H48" t="s">
-        <v>1396</v>
-      </c>
-      <c r="I48" t="s">
-        <v>1397</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B49" t="s">
         <v>1179</v>
@@ -7682,15 +7699,15 @@
         <v>1179</v>
       </c>
       <c r="H49" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="I49" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="B50" t="s">
         <v>1177</v>
@@ -7711,7 +7728,7 @@
         <v>1177</v>
       </c>
       <c r="H50" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="I50" t="s">
         <v>1178</v>
@@ -7719,7 +7736,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="B51" t="s">
         <v>1192</v>
@@ -7740,44 +7757,44 @@
         <v>1192</v>
       </c>
       <c r="H51" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I51" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1404</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1404</v>
+      </c>
+      <c r="H52" t="s">
+        <v>1405</v>
+      </c>
+      <c r="I52" t="s">
         <v>1406</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1407</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1407</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1407</v>
-      </c>
-      <c r="E52" t="s">
-        <v>1407</v>
-      </c>
-      <c r="F52" t="s">
-        <v>1407</v>
-      </c>
-      <c r="G52" t="s">
-        <v>1407</v>
-      </c>
-      <c r="H52" t="s">
-        <v>1408</v>
-      </c>
-      <c r="I52" t="s">
-        <v>1409</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="B53" t="s">
         <v>1195</v>
@@ -7798,7 +7815,7 @@
         <v>1195</v>
       </c>
       <c r="H53" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="I53" t="s">
         <v>1196</v>
@@ -7806,65 +7823,65 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1410</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1410</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1411</v>
+      </c>
+      <c r="I54" t="s">
         <v>1412</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1413</v>
-      </c>
-      <c r="D54" t="s">
-        <v>1413</v>
-      </c>
-      <c r="E54" t="s">
-        <v>1413</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1413</v>
-      </c>
-      <c r="G54" t="s">
-        <v>1413</v>
-      </c>
-      <c r="H54" t="s">
-        <v>1414</v>
-      </c>
-      <c r="I54" t="s">
-        <v>1415</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1414</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1414</v>
+      </c>
+      <c r="H55" t="s">
+        <v>1415</v>
+      </c>
+      <c r="I55" t="s">
         <v>1416</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1417</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1417</v>
-      </c>
-      <c r="D55" t="s">
-        <v>1417</v>
-      </c>
-      <c r="E55" t="s">
-        <v>1417</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1417</v>
-      </c>
-      <c r="G55" t="s">
-        <v>1417</v>
-      </c>
-      <c r="H55" t="s">
-        <v>1418</v>
-      </c>
-      <c r="I55" t="s">
-        <v>1419</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="B56" t="s">
         <v>1186</v>
@@ -7885,15 +7902,15 @@
         <v>1186</v>
       </c>
       <c r="H56" t="s">
-        <v>1421</v>
+        <v>1469</v>
       </c>
       <c r="I56" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="B57" t="s">
         <v>1189</v>
@@ -7914,7 +7931,7 @@
         <v>1189</v>
       </c>
       <c r="H57" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="I57" t="s">
         <v>1190</v>
@@ -7922,7 +7939,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="B58" t="s">
         <v>1181</v>
@@ -7943,15 +7960,15 @@
         <v>1181</v>
       </c>
       <c r="H58" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="I58" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="B59" t="s">
         <v>1183</v>
@@ -7972,15 +7989,15 @@
         <v>1183</v>
       </c>
       <c r="H59" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="I59" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
       <c r="B60" t="s">
         <v>1184</v>
@@ -8001,7 +8018,7 @@
         <v>1184</v>
       </c>
       <c r="H60" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
       <c r="I60" t="s">
         <v>1185</v>
@@ -8009,7 +8026,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="B61" t="s">
         <v>1193</v>
@@ -8030,7 +8047,7 @@
         <v>1193</v>
       </c>
       <c r="H61" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="I61" t="s">
         <v>1194</v>
@@ -8038,7 +8055,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="B62" t="s">
         <v>1187</v>
@@ -8059,7 +8076,7 @@
         <v>1187</v>
       </c>
       <c r="H62" t="s">
-        <v>1436</v>
+        <v>1432</v>
       </c>
       <c r="I62" t="s">
         <v>1188</v>
@@ -8067,36 +8084,36 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1434</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G63" t="s">
+        <v>1434</v>
+      </c>
+      <c r="H63" t="s">
+        <v>1436</v>
+      </c>
+      <c r="I63" t="s">
         <v>1437</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1438</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1439</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1438</v>
-      </c>
-      <c r="E63" t="s">
-        <v>1438</v>
-      </c>
-      <c r="F63" t="s">
-        <v>1438</v>
-      </c>
-      <c r="G63" t="s">
-        <v>1438</v>
-      </c>
-      <c r="H63" t="s">
-        <v>1440</v>
-      </c>
-      <c r="I63" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
       <c r="B64" t="s">
         <v>1182</v>
@@ -8117,44 +8134,44 @@
         <v>1182</v>
       </c>
       <c r="H64" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="I64" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="B65" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="C65" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="D65" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="E65" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="F65" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="G65" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="H65" t="s">
-        <v>1447</v>
+        <v>1443</v>
       </c>
       <c r="I65" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="B66" t="s">
         <v>1191</v>
@@ -8175,73 +8192,73 @@
         <v>1191</v>
       </c>
       <c r="H66" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="I66" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="B67" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="C67" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="D67" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="E67" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="F67" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="G67" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="H67" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
       <c r="I67" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="B68" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="C68" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="D68" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="E68" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="F68" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="G68" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="H68" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
       <c r="I68" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="B69" t="s">
         <v>1180</v>
@@ -8262,68 +8279,68 @@
         <v>1180</v>
       </c>
       <c r="H69" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="I69" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
       <c r="B70" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="C70" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="D70" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="E70" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="F70" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="G70" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="H70" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="I70" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="B71" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="C71" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="D71" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="E71" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="F71" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="G71" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="H71" t="s">
         <v>1209</v>
       </c>
       <c r="I71" t="s">
-        <v>1469</v>
+        <v>1465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bold final teams and non-bold third place teams
</commit_message>
<xml_diff>
--- a/src/stp/database/localization.xlsx
+++ b/src/stp/database/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B3FB7F-D59A-344F-B5AA-0FA235FB7F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3ED1B-AB03-0D41-A3F6-11600B66F023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="34200" windowHeight="19300" activeTab="2" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="34200" windowHeight="19300" activeTab="9" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Competition" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1471">
   <si>
     <t>key</t>
   </si>
@@ -4466,6 +4466,9 @@
   </si>
   <si>
     <t>ラザフォード、NJ</t>
+  </si>
+  <si>
+    <t>third.team.name</t>
   </si>
 </sst>
 </file>
@@ -4665,49 +4668,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4760,6 +4720,49 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -4902,7 +4905,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A92B97DC-54AE-2A49-B366-A6504207E4CF}" name="Venue" displayName="Venue" ref="A1:I71" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A92B97DC-54AE-2A49-B366-A6504207E4CF}" name="Venue" displayName="Venue" ref="A1:I71" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:I71" xr:uid="{A92B97DC-54AE-2A49-B366-A6504207E4CF}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B0B3E3B6-7AC0-B341-AA47-E0828ED515C1}" name="key"/>
@@ -4966,7 +4969,7 @@
     <tableColumn id="5" xr3:uid="{0318B88A-79B0-4BA8-931F-32E598CDDD83}" name="fr"/>
     <tableColumn id="6" xr3:uid="{7FB94F46-D9D6-4FFA-A68A-D9C22DD62960}" name="de"/>
     <tableColumn id="7" xr3:uid="{8DA7014B-3E29-4B6A-905E-FD5A34D770FA}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{21D35627-DEB2-4E21-A7A7-5800DA843F2D}" name="ja" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{21D35627-DEB2-4E21-A7A7-5800DA843F2D}" name="ja" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{0E0ECA8B-5B6D-4A0F-9BA3-F5F697D5FD39}" name="fa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5014,10 +5017,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I42" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I42" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="A1:I42" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{E3E8593F-CDB5-CA4C-B2DF-C5D167E6F581}" name="en"/>
     <tableColumn id="3" xr3:uid="{583B6CFD-84CD-BB44-88B6-0A0D3BA2E05E}" name="es"/>
     <tableColumn id="4" xr3:uid="{3139A9B8-E0C7-184A-8291-97B79E51FC05}" name="it"/>
@@ -5516,10 +5519,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5687,13 +5690,13 @@
         <v>1466</v>
       </c>
       <c r="B9" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="C9" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I9" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="J9" t="s">
         <v>672</v>
@@ -5935,6 +5938,23 @@
       </c>
       <c r="J23" t="s">
         <v>672</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B24" t="s">
+        <v>662</v>
+      </c>
+      <c r="C24" t="s">
+        <v>670</v>
+      </c>
+      <c r="I24" t="s">
+        <v>673</v>
+      </c>
+      <c r="J24" t="s">
+        <v>670</v>
       </c>
     </row>
   </sheetData>
@@ -6268,7 +6288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A607C59C-9131-3A41-BBFB-E38E1FFB1A83}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RtL dots; points dots leave room for total
</commit_message>
<xml_diff>
--- a/src/stp/database/localization.xlsx
+++ b/src/stp/database/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80819801-5582-4045-B89E-03ED3430F486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E301612A-3E6F-0141-9135-496D057F03C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="34200" windowHeight="19300" activeTab="9" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19300" activeTab="9" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Competition" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="1473">
   <si>
     <t>key</t>
   </si>
@@ -4472,6 +4472,9 @@
   </si>
   <si>
     <t>group.team.place</t>
+  </si>
+  <si>
+    <t>group.team.point-total</t>
   </si>
 </sst>
 </file>
@@ -4868,10 +4871,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J24" totalsRowShown="0">
-  <autoFilter ref="A1:J24" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J24">
-    <sortCondition ref="A1:A24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J25" totalsRowShown="0">
+  <autoFilter ref="A1:J25" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J25">
+    <sortCondition ref="A1:A25"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4614A9ED-E890-4F3B-BD19-53C40876125F}" name="key"/>
@@ -5522,10 +5525,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5843,58 +5846,58 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>650</v>
+        <v>1472</v>
       </c>
       <c r="B18" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="C18" t="s">
         <v>670</v>
       </c>
       <c r="I18" t="s">
-        <v>660</v>
+        <v>674</v>
       </c>
       <c r="J18" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1024</v>
+        <v>650</v>
       </c>
       <c r="B19" t="s">
-        <v>1025</v>
+        <v>660</v>
       </c>
       <c r="C19" t="s">
         <v>670</v>
       </c>
       <c r="I19" t="s">
-        <v>1025</v>
+        <v>660</v>
       </c>
       <c r="J19" t="s">
-        <v>1025</v>
+        <v>660</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>651</v>
+        <v>1024</v>
       </c>
       <c r="B20" t="s">
-        <v>665</v>
+        <v>1025</v>
       </c>
       <c r="C20" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I20" t="s">
-        <v>675</v>
+        <v>1025</v>
       </c>
       <c r="J20" t="s">
-        <v>672</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>693</v>
+        <v>651</v>
       </c>
       <c r="B21" t="s">
         <v>665</v>
@@ -5911,69 +5914,86 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>649</v>
+        <v>693</v>
       </c>
       <c r="B22" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="C22" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="I22" t="s">
-        <v>660</v>
+        <v>675</v>
       </c>
       <c r="J22" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B23" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C23" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="I23" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="J23" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
       <c r="B24" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C24" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J24" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>659</v>
+      </c>
+      <c r="B25" t="s">
+        <v>667</v>
+      </c>
+      <c r="C25" t="s">
+        <v>672</v>
+      </c>
+      <c r="I25" t="s">
+        <v>675</v>
+      </c>
+      <c r="J25" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>1470</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>662</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>670</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>673</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J26" t="s">
         <v>670</v>
       </c>
     </row>

</xml_diff>

<commit_message>
group total points in same font as ranking
</commit_message>
<xml_diff>
--- a/src/stp/database/localization.xlsx
+++ b/src/stp/database/localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E301612A-3E6F-0141-9135-496D057F03C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3668C513-6395-554B-9725-D61E9F37B706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19300" activeTab="9" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
@@ -5528,7 +5528,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5849,16 +5849,16 @@
         <v>1472</v>
       </c>
       <c r="B18" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C18" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="I18" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="J18" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
after extra time abbreviation (AET) in all languages
</commit_message>
<xml_diff>
--- a/src/stp/database/localization.xlsx
+++ b/src/stp/database/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3668C513-6395-554B-9725-D61E9F37B706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CD0A84-7C56-A644-A3BB-9BBDF23FF1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19300" activeTab="9" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19300" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Competition" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="1481">
   <si>
     <t>key</t>
   </si>
@@ -4475,6 +4475,30 @@
   </si>
   <si>
     <t>group.team.point-total</t>
+  </si>
+  <si>
+    <t>after-extra-time</t>
+  </si>
+  <si>
+    <t>(AET)</t>
+  </si>
+  <si>
+    <t>(DP)</t>
+  </si>
+  <si>
+    <t>(DTS)</t>
+  </si>
+  <si>
+    <t>(AP)</t>
+  </si>
+  <si>
+    <t>(NV)</t>
+  </si>
+  <si>
+    <t>(延長)</t>
+  </si>
+  <si>
+    <t>(و.ا)</t>
   </si>
 </sst>
 </file>
@@ -4983,8 +5007,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0574641-9580-4C09-8594-7E1FA61261E7}" name="Table5" displayName="Table5" ref="A1:J2" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{D0574641-9580-4C09-8594-7E1FA61261E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0574641-9580-4C09-8594-7E1FA61261E7}" name="Table5" displayName="Table5" ref="A1:J3" totalsRowShown="0">
+  <autoFilter ref="A1:J3" xr:uid="{D0574641-9580-4C09-8594-7E1FA61261E7}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F200773D-7393-4EE7-A925-5C77D146CD64}" name="key"/>
     <tableColumn id="2" xr3:uid="{9874EBD6-C206-4CB9-B976-F2D4FA230E33}" name="en"/>
@@ -5527,7 +5551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
+    <sheetView zoomScale="145" workbookViewId="0">
       <selection activeCell="B17" sqref="B17:J18"/>
     </sheetView>
   </sheetViews>
@@ -9026,10 +9050,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E988A0-3272-4A07-B301-DE09586F293E}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9099,6 +9123,35 @@
       </c>
       <c r="J2" t="s">
         <v>682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1478</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>